<commit_message>
cleanup & update readme.md
</commit_message>
<xml_diff>
--- a/nav-datasheet.xlsx
+++ b/nav-datasheet.xlsx
@@ -41,7 +41,7 @@
     <r>
       <rPr>
         <sz val="16"/>
-        <color indexed="11"/>
+        <color indexed="13"/>
         <rFont val="Times New Roman"/>
       </rPr>
       <t>8</t>
@@ -57,10 +57,10 @@
     <r>
       <rPr>
         <sz val="16"/>
-        <color indexed="11"/>
+        <color indexed="13"/>
         <rFont val="Times New Roman"/>
       </rPr>
-      <t>33</t>
+      <t>27</t>
     </r>
   </si>
   <si>
@@ -70,7 +70,7 @@
     <r>
       <rPr>
         <sz val="16"/>
-        <color indexed="11"/>
+        <color indexed="13"/>
         <rFont val="Times New Roman"/>
       </rPr>
       <t>A</t>
@@ -86,10 +86,10 @@
     <r>
       <rPr>
         <sz val="16"/>
-        <color indexed="11"/>
+        <color indexed="13"/>
         <rFont val="Times New Roman"/>
       </rPr>
-      <t> 27 September </t>
+      <t> 30 September </t>
     </r>
     <r>
       <rPr>
@@ -108,7 +108,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -116,6 +116,11 @@
     </font>
     <font>
       <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="13"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
@@ -132,11 +137,11 @@
     </font>
     <font>
       <sz val="16"/>
-      <color indexed="11"/>
+      <color indexed="13"/>
       <name val="Times New Roman"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -149,8 +154,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="12"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -177,14 +188,25 @@
       <left style="thin">
         <color indexed="9"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -193,28 +215,48 @@
         <color indexed="9"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="9"/>
       </right>
       <top style="thin">
         <color indexed="9"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="9"/>
       </left>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="9"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -224,29 +266,38 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -267,9 +318,10 @@
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="d8000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffffff00"/>
       <rgbColor rgb="ff1f497d"/>
-      <rgbColor rgb="ffa5a5a5"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -286,10 +338,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -466,11 +518,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:schemeClr val="accent1"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -479,27 +534,27 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
@@ -756,10 +811,10 @@
         <a:noFill/>
         <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1050,7 +1105,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1331,21 +1386,20 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="45.0625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="27.6172" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.125" style="1" customWidth="1"/>
-    <col min="4" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="45" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.6719" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.1719" style="1" customWidth="1"/>
+    <col min="4" max="5" width="16.3516" style="1" customWidth="1"/>
+    <col min="6" max="256" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="72.3" customHeight="1">
+    <row r="1" ht="56.05" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
@@ -1355,6 +1409,8 @@
       <c r="C1" t="s" s="2">
         <v>2</v>
       </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" ht="18.3" customHeight="1">
       <c r="A2" t="s" s="2">
@@ -1363,9 +1419,11 @@
       <c r="B2" t="s" s="2">
         <v>4</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="C2" t="s" s="5">
         <v>5</v>
       </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" ht="18.3" customHeight="1">
       <c r="A3" t="s" s="2">
@@ -1374,18 +1432,25 @@
       <c r="B3" t="s" s="2">
         <v>4</v>
       </c>
-      <c r="C3" s="4">
-        <v>0.9699</v>
+      <c r="C3" s="6">
+        <v>0.9654</v>
       </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="4"/>
     </row>
-    <row r="4" ht="20.35" customHeight="1">
-      <c r="A4" t="s" s="5">
+    <row r="4" ht="23.5" customHeight="1">
+      <c r="A4" t="s" s="7">
         <v>7</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A4:C4"/>
+  </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>

</xml_diff>

<commit_message>
fix source date undefined bug & nav value 4 decimal place bug
</commit_message>
<xml_diff>
--- a/nav-datasheet.xlsx
+++ b/nav-datasheet.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
   <si>
     <t>Fund Name</t>
   </si>
@@ -20,8 +20,10 @@
     <t>Currency Class</t>
   </si>
   <si>
-    <t>Latest NAV ( Currency as per Class )
-(Per Share)</t>
+    <t>Latest NAV</t>
+  </si>
+  <si>
+    <t>Source Date</t>
   </si>
   <si>
     <t>RHB Singapore Income Fund (RSIF)</t>
@@ -32,35 +34,37 @@
   <si>
     <r>
       <rPr>
-        <sz val="16"/>
+        <sz val="12"/>
         <color indexed="8"/>
-        <rFont val="Times New Roman"/>
+        <rFont val="Times"/>
       </rPr>
       <t>0.</t>
     </r>
     <r>
       <rPr>
-        <sz val="16"/>
-        <color indexed="13"/>
-        <rFont val="Times New Roman"/>
+        <sz val="12"/>
+        <color indexed="12"/>
+        <rFont val="Times"/>
       </rPr>
-      <t>8</t>
+      <t>82</t>
     </r>
     <r>
       <rPr>
-        <sz val="16"/>
+        <sz val="12"/>
         <color indexed="8"/>
-        <rFont val="Times New Roman"/>
+        <rFont val="Times"/>
       </rPr>
-      <t>3</t>
+      <t>45</t>
     </r>
+  </si>
+  <si>
     <r>
       <rPr>
-        <sz val="16"/>
-        <color indexed="13"/>
-        <rFont val="Times New Roman"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times"/>
       </rPr>
-      <t>27</t>
+      <t>As at 3 October 2019</t>
     </r>
   </si>
   <si>
@@ -69,35 +73,19 @@
   <si>
     <r>
       <rPr>
-        <sz val="16"/>
-        <color indexed="13"/>
-        <rFont val="Times New Roman"/>
+        <sz val="12"/>
+        <color indexed="12"/>
+        <rFont val="Times"/>
       </rPr>
-      <t>A</t>
+      <t>0.9</t>
     </r>
     <r>
       <rPr>
-        <sz val="16"/>
+        <sz val="12"/>
         <color indexed="8"/>
-        <rFont val="Times New Roman"/>
+        <rFont val="Times"/>
       </rPr>
-      <t>s at</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color indexed="13"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t> 30 September </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>2019</t>
+      <t>571</t>
     </r>
   </si>
 </sst>
@@ -126,19 +114,19 @@
     </font>
     <font>
       <b val="1"/>
-      <sz val="16"/>
+      <sz val="12"/>
       <color indexed="8"/>
-      <name val="Times New Roman"/>
+      <name val="Times"/>
     </font>
     <font>
-      <sz val="16"/>
+      <sz val="12"/>
       <color indexed="8"/>
-      <name val="Times New Roman"/>
+      <name val="Times"/>
     </font>
     <font>
-      <sz val="16"/>
-      <color indexed="13"/>
-      <name val="Times New Roman"/>
+      <sz val="12"/>
+      <color indexed="12"/>
+      <name val="Times"/>
     </font>
   </fonts>
   <fills count="4">
@@ -150,18 +138,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
+        <fgColor indexed="9"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="12"/>
+        <fgColor indexed="11"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -171,92 +159,116 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="8"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="8"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
+      <top/>
       <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="9"/>
-      </left>
-      <right style="thin">
-        <color indexed="9"/>
-      </right>
-      <top style="thin">
-        <color indexed="9"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="9"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="9"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="9"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -266,30 +278,33 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
@@ -298,6 +313,18 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -317,7 +344,6 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="d8000000"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffffff00"/>
@@ -1386,7 +1412,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1394,12 +1420,12 @@
   <cols>
     <col min="1" max="1" width="45" style="1" customWidth="1"/>
     <col min="2" max="2" width="27.6719" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.1719" style="1" customWidth="1"/>
-    <col min="4" max="5" width="16.3516" style="1" customWidth="1"/>
+    <col min="3" max="4" width="23.1719" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.3516" style="1" customWidth="1"/>
     <col min="6" max="256" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="56.05" customHeight="1">
+    <row r="1" ht="17" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
@@ -1409,47 +1435,91 @@
       <c r="C1" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4"/>
+      <c r="D1" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" ht="18.3" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s" s="5">
         <v>5</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4"/>
+      <c r="C2" t="s" s="4">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s" s="4">
+        <v>7</v>
+      </c>
+      <c r="E2" s="5"/>
     </row>
     <row r="3" ht="18.3" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
-      <c r="C3" s="6">
-        <v>0.9654</v>
+      <c r="C3" t="s" s="6">
+        <v>9</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="4"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="5"/>
     </row>
-    <row r="4" ht="23.5" customHeight="1">
-      <c r="A4" t="s" s="7">
-        <v>7</v>
-      </c>
-      <c r="B4" s="8"/>
+    <row r="4" ht="14.7" customHeight="1">
+      <c r="A4" s="8"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="9"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="4"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="10"/>
+    </row>
+    <row r="5" ht="14.7" customHeight="1">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="10"/>
+    </row>
+    <row r="6" ht="14.7" customHeight="1">
+      <c r="A6" s="11"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="10"/>
+    </row>
+    <row r="7" ht="14.7" customHeight="1">
+      <c r="A7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="10"/>
+    </row>
+    <row r="8" ht="14.7" customHeight="1">
+      <c r="A8" s="11"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="10"/>
+    </row>
+    <row r="9" ht="14.7" customHeight="1">
+      <c r="A9" s="11"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="10"/>
+    </row>
+    <row r="10" ht="14.7" customHeight="1">
+      <c r="A10" s="13"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D2:D3"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>